<commit_message>
Refactored transfer automation, TransferManager
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/downloads/Behlog Produce_IBProduce - Copy.xlsx
+++ b/WorkBot/main/backend/downloads/Behlog Produce_IBProduce - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\Andrew\Projects\RandomStuff\WorkBot\main\backend\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4385FAC5-7D78-4FD7-8AF4-5446D6D50F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C87B3BD-9F85-4C85-BECC-1DF84D07BB82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{EC4EC159-847C-4AEB-BECD-E328E488F5F3}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="12270" xr2:uid="{EC4EC159-847C-4AEB-BECD-E328E488F5F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>Case Size</t>
   </si>
@@ -105,9 +105,6 @@
     <t>2/5lb</t>
   </si>
   <si>
-    <t>case</t>
-  </si>
-  <si>
     <t>Kiwi</t>
   </si>
   <si>
@@ -228,6 +225,9 @@
     <t>Melon - Cantaloupe</t>
   </si>
   <si>
+    <t>Melon - Honeydew</t>
+  </si>
+  <si>
     <t>Melon - Watermelon</t>
   </si>
   <si>
@@ -303,7 +303,7 @@
     <t>Tomato - Grape</t>
   </si>
   <si>
-    <t>Item Name 1930 2/2/25</t>
+    <t>Item Name 1930 2/9/25</t>
   </si>
   <si>
     <t>1 cs</t>
@@ -727,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DC0EAE-FFF1-4108-95C9-562516A7BD65}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,7 @@
         <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -770,13 +770,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1">
         <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="7">
         <v>18.75</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1">
         <v>45</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1">
         <v>50</v>
@@ -821,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="6">
-        <v>39.75</v>
+        <v>29.75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1">
         <v>187</v>
@@ -896,7 +896,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1">
         <v>226</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1">
         <v>1250</v>
@@ -933,12 +933,12 @@
         <v>21</v>
       </c>
       <c r="D14" s="6">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1">
         <v>386</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1">
         <v>60</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1">
         <v>174</v>
@@ -980,7 +980,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1">
         <v>176</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1">
         <v>321</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1">
         <v>275</v>
@@ -1022,7 +1022,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1">
         <v>340</v>
@@ -1036,13 +1036,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1">
         <v>347</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="6">
         <v>25.75</v>
@@ -1050,13 +1050,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1">
         <v>385</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="6">
         <v>10.75</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1">
         <v>833</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1">
         <v>253</v>
@@ -1092,13 +1092,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1">
         <v>259</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="6">
         <v>23</v>
@@ -1106,13 +1106,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="1">
         <v>554</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="6">
         <v>29.75</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1">
         <v>251</v>
@@ -1134,13 +1134,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="1">
         <v>1305</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" s="6">
         <v>24.25</v>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1">
         <v>285</v>
@@ -1157,18 +1157,18 @@
         <v>18</v>
       </c>
       <c r="D30" s="6">
-        <v>34.25</v>
+        <v>44.25</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1">
         <v>1330</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="6">
         <v>39.75</v>
@@ -1176,13 +1176,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1">
         <v>1350</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" s="6">
         <v>18.75</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1">
         <v>1375</v>
@@ -1204,366 +1204,380 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1">
-        <v>1455</v>
+        <v>1425</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" s="6">
-        <v>11.5</v>
+        <v>33.75</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="1">
-        <v>390</v>
+        <v>1455</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="D35" s="6">
-        <v>22</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B36" s="1">
-        <v>404</v>
+        <v>390</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D36" s="6">
-        <v>16.649999999999999</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="1">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D37" s="6">
-        <v>23</v>
+        <v>16.649999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1">
-        <v>420</v>
+        <v>403</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D38" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1">
-        <v>244</v>
+        <v>420</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D39" s="6">
-        <v>29.75</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1">
-        <v>490</v>
+        <v>244</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D40" s="6">
-        <v>25.75</v>
+        <v>29.75</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" s="1">
-        <v>825</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="7">
-        <v>22</v>
+        <v>490</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="6">
+        <v>25.75</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" s="1">
-        <v>455</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="6">
-        <v>23.75</v>
+        <v>825</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="7">
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1">
-        <v>1605</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="7">
-        <v>69.75</v>
+        <v>455</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="6">
+        <v>23.75</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B44" s="1">
-        <v>828</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D44" s="6">
-        <v>38.75</v>
+        <v>1605</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="7">
+        <v>69.75</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="1">
+        <v>828</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" s="6">
+        <v>38.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B46" s="1">
         <v>563</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="6">
+      <c r="C46" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="6">
         <v>45.75</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B47" s="1">
         <v>570</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="6">
+      <c r="C47" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="6">
         <v>29.75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="1">
-        <v>565</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="6">
-        <v>27.75</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1">
-        <v>604</v>
+        <v>565</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D48" s="7">
-        <v>22.75</v>
+        <v>90</v>
+      </c>
+      <c r="D48" s="6">
+        <v>24.75</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1">
-        <v>575</v>
+        <v>604</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="6">
-        <v>26.75</v>
+        <v>31</v>
+      </c>
+      <c r="D49" s="7">
+        <v>22.75</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1">
-        <v>1655</v>
+        <v>575</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="D50" s="6">
-        <v>27.75</v>
+        <v>26.75</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="B51" s="1">
-        <v>690</v>
+        <v>1655</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="D51" s="6">
-        <v>15.5</v>
+        <v>27.75</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B52" s="1">
-        <v>660</v>
+        <v>690</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="6">
-        <v>22</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" s="1">
-        <v>735</v>
+        <v>660</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D53" s="6">
-        <v>20.75</v>
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="1">
-        <v>855</v>
-      </c>
-      <c r="C54" s="8" t="s">
+        <v>735</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D54" s="7">
-        <v>44.35</v>
+      <c r="D54" s="6">
+        <v>23.75</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="1">
-        <v>880</v>
+        <v>855</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D55" s="7">
-        <v>34.75</v>
+        <v>44.35</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="1">
-        <v>1150</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D56" s="6">
-        <v>34.65</v>
+        <v>880</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="7">
+        <v>34.75</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B57" s="1">
-        <v>920</v>
+        <v>1150</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="D57" s="6">
-        <v>24.75</v>
+        <v>34.75</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B58" s="1">
-        <v>931</v>
+        <v>920</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D58" s="6">
-        <v>19.5</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="B59" s="1">
+        <v>931</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" s="6">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B60" s="1">
         <v>865</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D59" s="6">
-        <v>31.45</v>
+      <c r="D60" s="6">
+        <v>28.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began refactoring CLI command registration
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/downloads/Behlog Produce_IBProduce - Copy.xlsx
+++ b/WorkBot/main/backend/downloads/Behlog Produce_IBProduce - Copy.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bljrdistribution-my.sharepoint.com/personal/luke_garris_behlogfs_com/Documents/Documents/Bids/Ithaca Bakery/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\Andrew\Projects\RandomStuff\WorkBot\main\backend\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{521728CD-CB76-4776-BF7A-DB646D1A107D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69C54D47-72C2-43CE-8A28-C7BC70067D3E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A93089-E424-4AFF-8760-7B5D9953A290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC4EC159-847C-4AEB-BECD-E328E488F5F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EC4EC159-847C-4AEB-BECD-E328E488F5F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>Case Size</t>
   </si>
@@ -44,30 +42,15 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Alfalfa Sprouts</t>
-  </si>
-  <si>
     <t>3lb</t>
   </si>
   <si>
-    <t>Apple Cider</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>12/3lb</t>
-  </si>
-  <si>
     <t>Bananas</t>
   </si>
   <si>
     <t>40lb</t>
   </si>
   <si>
-    <t>crate</t>
-  </si>
-  <si>
     <t>20lb</t>
   </si>
   <si>
@@ -110,9 +93,6 @@
     <t>12ct</t>
   </si>
   <si>
-    <t>30dz</t>
-  </si>
-  <si>
     <t>4/5lb</t>
   </si>
   <si>
@@ -122,18 +102,9 @@
     <t>18lb</t>
   </si>
   <si>
-    <t>Green Beans</t>
-  </si>
-  <si>
-    <t>Green Beans (Trimmed &amp; Fresh)</t>
-  </si>
-  <si>
     <t>2/5lb</t>
   </si>
   <si>
-    <t>case</t>
-  </si>
-  <si>
     <t>Kiwi</t>
   </si>
   <si>
@@ -173,12 +144,6 @@
     <t>Pineapple</t>
   </si>
   <si>
-    <t>Radish</t>
-  </si>
-  <si>
-    <t>60/5oz</t>
-  </si>
-  <si>
     <t>12/3ct</t>
   </si>
   <si>
@@ -188,21 +153,12 @@
     <t>12/pt</t>
   </si>
   <si>
-    <t>each</t>
-  </si>
-  <si>
     <t>Zucchini Fancy Medium</t>
   </si>
   <si>
     <t>Item SKU</t>
   </si>
   <si>
-    <t xml:space="preserve">Apple - Empire </t>
-  </si>
-  <si>
-    <t>6/1G</t>
-  </si>
-  <si>
     <t>Beets</t>
   </si>
   <si>
@@ -218,27 +174,15 @@
     <t>Cucumbers (English)</t>
   </si>
   <si>
-    <t>Eggs (Shell-On)</t>
-  </si>
-  <si>
     <t>Garlic (Peeled)</t>
   </si>
   <si>
     <t>Grapes - Red (Seedless)</t>
   </si>
   <si>
-    <t>Crate</t>
-  </si>
-  <si>
     <t>Greens - Arugula (Baby)</t>
   </si>
   <si>
-    <t>Greens - Bok Choy</t>
-  </si>
-  <si>
-    <t>sp</t>
-  </si>
-  <si>
     <t>Greens - Cabbage (NAPA)</t>
   </si>
   <si>
@@ -251,18 +195,9 @@
     <t>Greens - Green Leaf Lettuce (Fillet)</t>
   </si>
   <si>
-    <t>Greens - Green Leaf Lettuce (Washed &amp; Trimmed)</t>
-  </si>
-  <si>
     <t>Greens - Kale</t>
   </si>
   <si>
-    <t>Greens - Kale (Cleaned)</t>
-  </si>
-  <si>
-    <t>Greens - Rapini (Broccoli Rabe)</t>
-  </si>
-  <si>
     <t>Greens - Romaine (Hearts)</t>
   </si>
   <si>
@@ -275,12 +210,6 @@
     <t>Greens - Spinach (Baby)</t>
   </si>
   <si>
-    <t>Greens - Spring Mix</t>
-  </si>
-  <si>
-    <t>Greens - Swiss Chard</t>
-  </si>
-  <si>
     <t>Herb - Cilantro</t>
   </si>
   <si>
@@ -290,9 +219,6 @@
     <t>Herb - Parsley</t>
   </si>
   <si>
-    <t>Herb - Parsley (Washed &amp; Trimmed)</t>
-  </si>
-  <si>
     <t>Herbs - Basil (Cleaned)</t>
   </si>
   <si>
@@ -323,18 +249,12 @@
     <t>Onion - Red</t>
   </si>
   <si>
-    <t>Onion - Red (Peeled)</t>
-  </si>
-  <si>
     <t>Onion - Shallot Peeled</t>
   </si>
   <si>
     <t>Onion - Spanish</t>
   </si>
   <si>
-    <t>Onion - Spanish (Peeled)</t>
-  </si>
-  <si>
     <t>Pears</t>
   </si>
   <si>
@@ -356,21 +276,6 @@
     <t>Pepper - Red Bell (11 LB)</t>
   </si>
   <si>
-    <t>Pepper - Red Bell (25 LB)</t>
-  </si>
-  <si>
-    <t>bushel</t>
-  </si>
-  <si>
-    <t>Pepper - Red Bell (5 LB)</t>
-  </si>
-  <si>
-    <t>Pomegranate (Whole)</t>
-  </si>
-  <si>
-    <t>Pomegranate Seeds (Frozen)</t>
-  </si>
-  <si>
     <t>Potato - Chef</t>
   </si>
   <si>
@@ -398,10 +303,13 @@
     <t>Tomato - Grape</t>
   </si>
   <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>Item Name 1930 4/6/25</t>
+    <t>Item Name 1930 3/23/25</t>
+  </si>
+  <si>
+    <t>1 cs</t>
+  </si>
+  <si>
+    <t>1 ea</t>
   </si>
 </sst>
 </file>
@@ -434,7 +342,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -472,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -481,12 +388,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -821,9 +727,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DC0EAE-FFF1-4108-95C9-562516A7BD65}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -834,10 +742,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -848,1058 +756,828 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>845</v>
+        <v>1125</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D2" s="6">
+        <v>23.75</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1">
-        <v>1096</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
+      </c>
+      <c r="D3" s="7">
+        <v>18.75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1">
-        <v>1081</v>
+        <v>45</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>25.75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1">
-        <v>1125</v>
+        <v>50</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="7">
-        <v>23.75</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="6">
+        <v>36.75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="8">
-        <v>18.75</v>
+        <v>8</v>
+      </c>
+      <c r="D6" s="6">
+        <v>30.75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="7">
-        <v>25.75</v>
+        <v>8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>21.65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7">
-        <v>36.75</v>
+        <v>9</v>
+      </c>
+      <c r="D8" s="6">
+        <v>28.75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="7">
-        <v>30.75</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="6">
+        <v>26.75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="7">
-        <v>21.65</v>
+        <v>15</v>
+      </c>
+      <c r="D10" s="6">
+        <v>33.75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1">
-        <v>82</v>
+        <v>187</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="7">
-        <v>26.75</v>
+        <v>18</v>
+      </c>
+      <c r="D11" s="6">
+        <v>19.75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1">
-        <v>125</v>
+        <v>226</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="7">
-        <v>26.75</v>
+        <v>19</v>
+      </c>
+      <c r="D12" s="6">
+        <v>74.75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>141</v>
+        <v>237</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="7">
-        <v>33.75</v>
+        <v>17</v>
+      </c>
+      <c r="D13" s="6">
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1">
-        <v>187</v>
+        <v>1250</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="7">
-        <v>19.75</v>
+        <v>21</v>
+      </c>
+      <c r="D14" s="6">
+        <v>32.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1">
-        <v>1870</v>
+        <v>386</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>120</v>
+        <v>2</v>
+      </c>
+      <c r="D15" s="6">
+        <v>25.75</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B16" s="1">
-        <v>226</v>
+        <v>60</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="7">
-        <v>74.75</v>
+        <v>9</v>
+      </c>
+      <c r="D16" s="6">
+        <v>46.75</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1">
-        <v>237</v>
+        <v>174</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="7">
-        <v>62</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B18" s="1">
-        <v>1250</v>
+        <v>176</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="7">
-        <v>32.5</v>
+        <v>17</v>
+      </c>
+      <c r="D18" s="6">
+        <v>22.75</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B19" s="1">
+        <v>321</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>5</v>
+      <c r="D19" s="6">
+        <v>29.25</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1">
-        <v>14</v>
+        <v>275</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>5</v>
+        <v>90</v>
+      </c>
+      <c r="D20" s="6">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1">
-        <v>386</v>
+        <v>340</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21" s="7">
-        <v>23.75</v>
+        <v>90</v>
+      </c>
+      <c r="D21" s="6">
+        <v>29.15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1">
-        <v>31</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="9" t="s">
-        <v>66</v>
+        <v>347</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="6">
+        <v>28.75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1">
-        <v>60</v>
+        <v>385</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="7">
-        <v>46.75</v>
+        <v>37</v>
+      </c>
+      <c r="D23" s="6">
+        <v>10.75</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1">
-        <v>174</v>
+        <v>833</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="8">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="D24" s="6">
+        <v>16.25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1">
-        <v>176</v>
+        <v>253</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="7">
-        <v>22.75</v>
+        <v>16</v>
+      </c>
+      <c r="D25" s="6">
+        <v>29.75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1">
-        <v>321</v>
+        <v>259</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="7">
-        <v>29.25</v>
+        <v>30</v>
+      </c>
+      <c r="D26" s="6">
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="B27" s="1">
+        <v>554</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="6">
+        <v>29.75</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B28" s="1">
-        <v>275</v>
+        <v>251</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="7">
-        <v>26</v>
+        <v>90</v>
+      </c>
+      <c r="D28" s="6">
+        <v>29.5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1305</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="6">
+        <v>24.25</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1">
-        <v>51</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>66</v>
+        <v>285</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="6">
+        <v>44.25</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1">
-        <v>340</v>
+        <v>1330</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="7">
-        <v>33.25</v>
+        <v>27</v>
+      </c>
+      <c r="D31" s="6">
+        <v>32.75</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1">
-        <v>347</v>
+        <v>1350</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D32" s="7">
-        <v>28.75</v>
+        <v>29</v>
+      </c>
+      <c r="D32" s="6">
+        <v>20.5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1">
-        <v>385</v>
+        <v>1375</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="7">
-        <v>10.75</v>
+        <v>10</v>
+      </c>
+      <c r="D33" s="6">
+        <v>28.75</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1">
-        <v>833</v>
+        <v>1425</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="7">
-        <v>16.25</v>
+        <v>90</v>
+      </c>
+      <c r="D34" s="6">
+        <v>27.45</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1455</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="6">
+        <v>11.5</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="B36" s="1">
+        <v>390</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="6">
+        <v>22</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B37" s="1">
-        <v>253</v>
+        <v>404</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="7">
-        <v>29.75</v>
+        <v>30</v>
+      </c>
+      <c r="D37" s="6">
+        <v>16.649999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1">
-        <v>259</v>
+        <v>403</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="7">
+        <v>2</v>
+      </c>
+      <c r="D38" s="6">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1">
-        <v>554</v>
+        <v>420</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="7">
-        <v>29.75</v>
+        <v>31</v>
+      </c>
+      <c r="D39" s="6">
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B40" s="1">
-        <v>556</v>
+        <v>244</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="D40" s="6">
+        <v>25.75</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B41" s="1">
-        <v>251</v>
+        <v>490</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="7">
-        <v>29.5</v>
+        <v>8</v>
+      </c>
+      <c r="D41" s="6">
+        <v>25.75</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B42" s="1">
-        <v>1305</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>33</v>
+        <v>825</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D42" s="7">
-        <v>24.25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B43" s="1">
-        <v>285</v>
+        <v>455</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="7">
-        <v>44.25</v>
+        <v>9</v>
+      </c>
+      <c r="D43" s="6">
+        <v>23.75</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B44" s="1">
-        <v>1330</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>36</v>
+        <v>1605</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="D44" s="7">
-        <v>32.75</v>
+        <v>69.75</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="B45" s="1">
-        <v>1350</v>
+        <v>828</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="7">
-        <v>20.5</v>
+        <v>31</v>
+      </c>
+      <c r="D45" s="6">
+        <v>29.5</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B46" s="1">
-        <v>1375</v>
+        <v>563</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="7">
-        <v>28.75</v>
+        <v>31</v>
+      </c>
+      <c r="D46" s="6">
+        <v>45.75</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>87</v>
+      <c r="A47" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B47" s="1">
-        <v>1425</v>
+        <v>570</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="7">
-        <v>24.45</v>
+        <v>90</v>
+      </c>
+      <c r="D47" s="6">
+        <v>31.75</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B48" s="1">
-        <v>1455</v>
+        <v>565</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="7">
-        <v>11.5</v>
+        <v>90</v>
+      </c>
+      <c r="D48" s="6">
+        <v>29.15</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1">
-        <v>390</v>
+        <v>604</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D49" s="7">
-        <v>22</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1">
-        <v>404</v>
+        <v>575</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="7">
-        <v>16.649999999999999</v>
+        <v>34</v>
+      </c>
+      <c r="D50" s="6">
+        <v>34.549999999999997</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B51" s="1">
-        <v>403</v>
+        <v>1655</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="7">
-        <v>23</v>
+        <v>90</v>
+      </c>
+      <c r="D51" s="6">
+        <v>28.25</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B52" s="1">
-        <v>420</v>
+        <v>690</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D52" s="7">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="D52" s="6">
+        <v>15.5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B53" s="1">
-        <v>244</v>
+        <v>660</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D53" s="7">
-        <v>25.75</v>
+        <v>9</v>
+      </c>
+      <c r="D53" s="6">
+        <v>23.75</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B54" s="1">
-        <v>490</v>
+        <v>735</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D54" s="7">
+        <v>9</v>
+      </c>
+      <c r="D54" s="6">
         <v>25.75</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B55" s="1">
-        <v>505</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>5</v>
+        <v>855</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="7">
+        <v>33.5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B56" s="1">
-        <v>825</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D56" s="8">
-        <v>22</v>
+        <v>880</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="7">
+        <v>31.4</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B57" s="1">
-        <v>455</v>
+        <v>1150</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D57" s="7">
-        <v>23.75</v>
+        <v>86</v>
+      </c>
+      <c r="D57" s="6">
+        <v>23.5</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B58" s="1">
-        <v>500</v>
+        <v>920</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D58" s="6">
+        <v>27.35</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B59" s="1">
-        <v>1605</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="8">
-        <v>69.75</v>
+        <v>931</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" s="6">
+        <v>19.5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
       <c r="B60" s="1">
-        <v>828</v>
+        <v>865</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D60" s="7">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B61" s="1">
-        <v>563</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D61" s="7">
-        <v>45.75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B62" s="1">
-        <v>570</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D62" s="7">
-        <v>31.75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B63" s="1">
-        <v>565</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D63" s="7">
-        <v>27.25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B64" s="1">
-        <v>604</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D64" s="8">
-        <v>22.75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B65" s="1">
-        <v>575</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D65" s="7">
-        <v>24.75</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B66" s="1">
-        <v>585</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="1"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B68" s="1">
-        <v>1655</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D68" s="7">
-        <v>28.25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B69" s="1"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="1"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="1"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B71" s="1">
-        <v>690</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D71" s="7">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B72" s="1">
-        <v>660</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="7">
-        <v>23.75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B73" s="1">
-        <v>735</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D73" s="7">
-        <v>25.75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B74" s="1">
-        <v>805</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D74" s="1"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B75" s="1">
-        <v>855</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="8">
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B76" s="1">
-        <v>880</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D76" s="8">
-        <v>31.4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B77" s="1">
-        <v>1150</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D77" s="7">
-        <v>25.25</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B78" s="1">
-        <v>920</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D78" s="7">
-        <v>28.75</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B79" s="1">
-        <v>931</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="7">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B80" s="1">
-        <v>865</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D80" s="7">
-        <v>20.25</v>
+        <v>90</v>
+      </c>
+      <c r="D60" s="6">
+        <v>24.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>